<commit_message>
Added column labels for cartesian/polar matrices
</commit_message>
<xml_diff>
--- a/ColumnLabels.xlsx
+++ b/ColumnLabels.xlsx
@@ -5,19 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="601" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="948" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FullLabels" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="withoutExtraneous" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="polarMatrix" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="cartesianMatrix" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
   <si>
     <t>user ID</t>
   </si>
@@ -325,8 +327,8 @@
   </sheetPr>
   <dimension ref="A1:A56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -716,7 +718,7 @@
   </sheetPr>
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -990,4 +992,350 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A26"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A32"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3724696356275"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Big update with decision tree
</commit_message>
<xml_diff>
--- a/ColumnLabels.xlsx
+++ b/ColumnLabels.xlsx
@@ -5,218 +5,285 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="948" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="FullLabels" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="withoutExtraneous" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="polarMatrix" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="cartesianMatrix" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="cartMat.mat" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="polarMat.mat" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="extendFeat.mat" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
-  <si>
-    <t>user ID</t>
-  </si>
-  <si>
-    <t>doc ID</t>
-  </si>
-  <si>
-    <t>inter-stroke time</t>
-  </si>
-  <si>
-    <t>stroke duration</t>
-  </si>
-  <si>
-    <t>start x</t>
-  </si>
-  <si>
-    <t>start y</t>
-  </si>
-  <si>
-    <t>stop x</t>
-  </si>
-  <si>
-    <t>stop y</t>
-  </si>
-  <si>
-    <t>direct end-to-end distance</t>
-  </si>
-  <si>
-    <t>mean resultant length</t>
-  </si>
-  <si>
-    <t>up/down/left/right flag</t>
-  </si>
-  <si>
-    <t>direction of end-to-end line</t>
-  </si>
-  <si>
-    <t>phone id</t>
-  </si>
-  <si>
-    <t>20 percent pairwise velocity</t>
-  </si>
-  <si>
-    <t>50 percent pairwaise velocity</t>
-  </si>
-  <si>
-    <t>80 percent pairwise veolcity</t>
-  </si>
-  <si>
-    <t>20 percent pairwise acceleration</t>
-  </si>
-  <si>
-    <t>50 percent pairwise acceleration</t>
-  </si>
-  <si>
-    <t>80 percent pairwise acceleration</t>
-  </si>
-  <si>
-    <t>median veolcity at last 3 point</t>
-  </si>
-  <si>
-    <t>largest deviation from end-to-end line</t>
-  </si>
-  <si>
-    <t>20 percent deviation from end-to-end line</t>
-  </si>
-  <si>
-    <t>50 percent deviation from end-to-end line</t>
-  </si>
-  <si>
-    <t>80 percent deviation from end-to-end line</t>
-  </si>
-  <si>
-    <t>average direction</t>
-  </si>
-  <si>
-    <t>length of trajectory</t>
-  </si>
-  <si>
-    <t>ratio end-to-end distance and length of trajectory</t>
-  </si>
-  <si>
-    <t>average velocity</t>
-  </si>
-  <si>
-    <t>median acceleration at first 5 points</t>
-  </si>
-  <si>
-    <t>mid-stroke pressure</t>
-  </si>
-  <si>
-    <t>mid-stroke area covered</t>
-  </si>
-  <si>
-    <t>mid-stroke finger orientation</t>
-  </si>
-  <si>
-    <t>change of finger orientation</t>
-  </si>
-  <si>
-    <t>phone orientation</t>
-  </si>
-  <si>
-    <t>rho start</t>
-  </si>
-  <si>
-    <t>theta start</t>
-  </si>
-  <si>
-    <t>rho end</t>
-  </si>
-  <si>
-    <t>theta end</t>
-  </si>
-  <si>
-    <t>20 percent drho/dt</t>
-  </si>
-  <si>
-    <t>50 percent drho/dt</t>
-  </si>
-  <si>
-    <t>80 percent drho/dt</t>
-  </si>
-  <si>
-    <t>20 percent dtheta/dt</t>
-  </si>
-  <si>
-    <t>50 percent dtheta/dt</t>
-  </si>
-  <si>
-    <t>80 percent dtheta/dt</t>
-  </si>
-  <si>
-    <t>20 percent d^2rho/dt^2</t>
-  </si>
-  <si>
-    <t>50 percent d^2rho/dt^2</t>
-  </si>
-  <si>
-    <t>80 percent d^2rho/dt^2</t>
-  </si>
-  <si>
-    <t>20 percent d^2theta/dt^2</t>
-  </si>
-  <si>
-    <t>50 percent d^2theta/dt^2</t>
-  </si>
-  <si>
-    <t>80 percent d^2theta/dt^2</t>
-  </si>
-  <si>
-    <t>median drho/dt at last 3 point</t>
-  </si>
-  <si>
-    <t>median dtheta/dt at last 3 point</t>
-  </si>
-  <si>
-    <t>x-displacment</t>
-  </si>
-  <si>
-    <t>y-displacement</t>
-  </si>
-  <si>
-    <t>rho-displacement</t>
-  </si>
-  <si>
-    <t>theta-displacement</t>
-  </si>
-  <si>
-    <t>Phone ID</t>
-  </si>
-  <si>
-    <t>User ID</t>
-  </si>
-  <si>
-    <t>Document ID</t>
-  </si>
-  <si>
-    <t>time (ms)</t>
-  </si>
-  <si>
-    <t>action</t>
-  </si>
-  <si>
-    <t>x-coordinate</t>
-  </si>
-  <si>
-    <t>y-coordinate</t>
-  </si>
-  <si>
-    <t>pressure</t>
-  </si>
-  <si>
-    <t>area covered</t>
-  </si>
-  <si>
-    <t>finger orientation</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="86">
+  <si>
+    <t xml:space="preserve">user ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doc ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inter-stroke time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stroke duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direct end-to-end distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean resultant length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">up/down/left/right flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direction of end-to-end line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 percent pairwise velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 percent pairwaise velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80 percent pairwise veolcity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 percent pairwise acceleration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 percent pairwise acceleration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80 percent pairwise acceleration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median veolcity at last 3 point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">largest deviation from end-to-end line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 percent deviation from end-to-end line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 percent deviation from end-to-end line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80 percent deviation from end-to-end line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">length of trajectory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratio end-to-end distance and length of trajectory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median acceleration at first 5 points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mid-stroke pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mid-stroke area covered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mid-stroke finger orientation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change of finger orientation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone orientation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rho start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">theta start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rho end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">theta end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 percent drho/dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 percent drho/dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80 percent drho/dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 percent dtheta/dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 percent dtheta/dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80 percent dtheta/dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 percent d^2rho/dt^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 percent d^2rho/dt^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80 percent d^2rho/dt^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 percent d^2theta/dt^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 percent d^2theta/dt^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80 percent d^2theta/dt^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median drho/dt at last 3 point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median dtheta/dt at last 3 point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x-displacment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y-displacement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rho-displacement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">theta-displacement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time (ms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x-coordinate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y-coordinate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">area covered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finger orientation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid-stroke pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid-stroke area covered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">theta start </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20% drho/dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% drho/dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80% drho/dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20% dtheta/dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% dtheta/dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80% dtheta/dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20% d^2rho/dt^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% d^2rho/dt^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80% d^2rho/dt^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20% d^2theta/dt^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% d^2theta/dt^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80% d^2theta/dt^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median drho/dt of last 3 points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">media dtheta/dt of last 3 points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rho-displacement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theta-displacement</t>
   </si>
 </sst>
 </file>
@@ -224,7 +291,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -327,14 +394,14 @@
   </sheetPr>
   <dimension ref="A1:A56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="8.88259109311741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,13 +703,13 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A1:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="8.88259109311741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -719,13 +786,13 @@
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
+      <selection pane="topLeft" activeCell="E40" activeCellId="1" sqref="A1:A52 E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.8704453441296"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1001,14 +1068,14 @@
   </sheetPr>
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D29" activeCellId="1" sqref="A1:A52 D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5951417004049"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.219387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,13 +1227,13 @@
   <dimension ref="A1:A32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="1" sqref="A1:A52 D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3724696356275"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,6 +1394,453 @@
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A1:A52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A52"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>